<commit_message>
new xlsx with fixed col names
</commit_message>
<xml_diff>
--- a/data/Moser creek data.xlsx
+++ b/data/Moser creek data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="95">
   <si>
     <t>3 sites moser creek</t>
   </si>
@@ -55,49 +55,49 @@
     <t>e + mv: edge with midvein</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>id</t>
   </si>
   <si>
-    <t>#Collinsia</t>
+    <t>Collinsia_count</t>
   </si>
   <si>
-    <t>Collinsia cover %</t>
+    <t>Collinsia_percentcover</t>
   </si>
   <si>
-    <t>Other plant cover %</t>
+    <t>otherplant_cover</t>
   </si>
   <si>
-    <t>Moss cover %</t>
+    <t>moss_cover</t>
   </si>
   <si>
-    <t xml:space="preserve">Rock cover % </t>
+    <t>rock_cover</t>
   </si>
   <si>
-    <t>Soil/ bare ground %</t>
+    <t>soilbareground_cover</t>
   </si>
   <si>
-    <t>Height cm</t>
+    <t>height_cm</t>
   </si>
   <si>
-    <t>leaves</t>
+    <t>leaf_count</t>
   </si>
   <si>
-    <t>flowers</t>
+    <t>flower_count</t>
   </si>
   <si>
-    <t>fruits</t>
+    <t>fruit_count</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>TRT</t>
+    <t>trt</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>date</t>
   </si>
   <si>
-    <t>Site</t>
+    <t>site</t>
   </si>
   <si>
     <t>C0</t>
@@ -196,10 +196,7 @@
     <t>herbivory 13.33% node 1 edge + MV</t>
   </si>
   <si>
-    <t>diameter</t>
-  </si>
-  <si>
-    <t>#Collinsia count</t>
+    <t>diameter_cm</t>
   </si>
   <si>
     <t>6.19.2025</t>
@@ -208,34 +205,16 @@
     <t>dead</t>
   </si>
   <si>
-    <t>Height</t>
+    <t>herbivory_percent</t>
   </si>
   <si>
-    <t>Diam</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>fl</t>
-  </si>
-  <si>
-    <t>lvs</t>
-  </si>
-  <si>
-    <t>herbivory %</t>
-  </si>
-  <si>
-    <t>Herb type</t>
+    <t>herbivory_type</t>
   </si>
   <si>
     <t>node</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>EFN score</t>
+    <t>EFN_score</t>
   </si>
   <si>
     <t>e no mv</t>
@@ -5307,7 +5286,7 @@
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
@@ -5376,7 +5355,7 @@
         <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
@@ -5421,7 +5400,7 @@
         <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
@@ -5466,7 +5445,7 @@
         <v>31</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
@@ -5511,7 +5490,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -5556,7 +5535,7 @@
         <v>38</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -5601,7 +5580,7 @@
         <v>34</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -5646,7 +5625,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
@@ -5691,7 +5670,7 @@
         <v>37</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
@@ -5736,7 +5715,7 @@
         <v>35</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
@@ -5781,7 +5760,7 @@
         <v>36</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -5826,7 +5805,7 @@
         <v>41</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -5871,7 +5850,7 @@
         <v>42</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -5916,7 +5895,7 @@
         <v>43</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
@@ -5961,7 +5940,7 @@
         <v>45</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
@@ -6006,7 +5985,7 @@
         <v>50</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
@@ -6051,7 +6030,7 @@
         <v>28</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18">
@@ -6096,7 +6075,7 @@
         <v>35</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
@@ -6141,7 +6120,7 @@
         <v>34</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
@@ -6186,7 +6165,7 @@
         <v>46</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21">
@@ -6231,7 +6210,7 @@
         <v>32</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22">
@@ -6276,7 +6255,7 @@
         <v>40</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
@@ -6321,7 +6300,7 @@
         <v>37</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
@@ -6366,7 +6345,7 @@
         <v>42</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25">
@@ -6411,7 +6390,7 @@
         <v>49</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26">
@@ -6456,7 +6435,7 @@
         <v>44</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27">
@@ -6501,7 +6480,7 @@
         <v>45</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28">
@@ -6546,7 +6525,7 @@
         <v>41</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
@@ -6591,7 +6570,7 @@
         <v>39</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30">
@@ -6636,7 +6615,7 @@
         <v>48</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31">
@@ -6681,7 +6660,7 @@
         <v>33</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32">
@@ -6726,7 +6705,7 @@
         <v>31</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33">
@@ -6771,7 +6750,7 @@
         <v>44</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34">
@@ -6816,7 +6795,7 @@
         <v>39</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35">
@@ -6861,7 +6840,7 @@
         <v>40</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36">
@@ -6906,7 +6885,7 @@
         <v>28</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37">
@@ -6951,7 +6930,7 @@
         <v>32</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38">
@@ -6996,7 +6975,7 @@
         <v>43</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39">
@@ -7041,7 +7020,7 @@
         <v>47</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40">
@@ -7086,7 +7065,7 @@
         <v>30</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41">
@@ -7131,7 +7110,7 @@
         <v>38</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42">
@@ -7176,7 +7155,7 @@
         <v>36</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43">
@@ -7221,7 +7200,7 @@
         <v>34</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44">
@@ -7266,7 +7245,7 @@
         <v>49</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45">
@@ -7311,7 +7290,7 @@
         <v>50</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46">
@@ -7356,7 +7335,7 @@
         <v>46</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47">
@@ -7401,7 +7380,7 @@
         <v>30</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48">
@@ -7446,7 +7425,7 @@
         <v>38</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49">
@@ -7491,7 +7470,7 @@
         <v>35</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50">
@@ -7536,7 +7515,7 @@
         <v>37</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51">
@@ -7581,7 +7560,7 @@
         <v>45</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52">
@@ -7626,7 +7605,7 @@
         <v>39</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53">
@@ -7671,7 +7650,7 @@
         <v>40</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54">
@@ -7716,7 +7695,7 @@
         <v>45</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55">
@@ -7761,7 +7740,7 @@
         <v>42</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56">
@@ -7806,7 +7785,7 @@
         <v>46</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57">
@@ -7851,7 +7830,7 @@
         <v>41</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58">
@@ -7896,7 +7875,7 @@
         <v>44</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59">
@@ -7941,7 +7920,7 @@
         <v>47</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60">
@@ -7986,7 +7965,7 @@
         <v>48</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61">
@@ -8031,7 +8010,7 @@
         <v>49</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62">
@@ -8076,7 +8055,7 @@
         <v>50</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63">
@@ -8121,7 +8100,7 @@
         <v>28</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64">
@@ -8166,7 +8145,7 @@
         <v>33</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65">
@@ -8211,7 +8190,7 @@
         <v>31</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66">
@@ -8256,7 +8235,7 @@
         <v>32</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67">
@@ -8264,13 +8243,13 @@
         <v>728.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68">
@@ -8278,13 +8257,13 @@
         <v>271.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69">
@@ -8292,13 +8271,13 @@
         <v>811.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>48</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70">
@@ -8306,13 +8285,13 @@
         <v>277.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>47</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71">
@@ -8320,13 +8299,13 @@
         <v>910.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -8352,37 +8331,37 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
@@ -8434,7 +8413,7 @@
         <v>1.875</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I3" s="1">
         <v>2.0</v>
@@ -8451,7 +8430,7 @@
         <v>728.0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="K4" s="3">
         <v>45833.0</v>
@@ -8584,7 +8563,7 @@
         <v>0.625</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I9" s="1">
         <v>3.0</v>
@@ -8720,7 +8699,7 @@
         <v>4.0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K14" s="3">
         <v>45833.0</v>
@@ -8786,7 +8765,7 @@
         <v>809.0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K17" s="3">
         <v>45833.0</v>
@@ -8797,7 +8776,7 @@
         <v>784.0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K18" s="3">
         <v>45833.0</v>
@@ -8901,7 +8880,7 @@
         <v>5.0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K22" s="3">
         <v>45833.0</v>
@@ -8915,7 +8894,7 @@
         <v>830.0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K23" s="3">
         <v>45833.0</v>
@@ -9308,7 +9287,7 @@
         <v>0.2</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I38" s="1">
         <v>3.0</v>
@@ -9525,7 +9504,7 @@
         <v>0.5</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I46" s="1">
         <v>1.0</v>
@@ -9560,10 +9539,10 @@
         <v>1.583</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="K47" s="3">
         <v>45833.0</v>
@@ -9595,7 +9574,7 @@
         <v>0.83</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I48" s="1">
         <v>1.0</v>
@@ -10069,7 +10048,7 @@
         <v>0.0</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K66" s="3">
         <v>45833.0</v>
@@ -10150,7 +10129,7 @@
         <v>6.0</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K69" s="3">
         <v>45833.0</v>
@@ -10182,10 +10161,10 @@
         <v>0.875</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="K70" s="3">
         <v>45833.0</v>
@@ -10329,7 +10308,7 @@
         <v>622.0</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K76" s="3">
         <v>45833.0</v>
@@ -10384,10 +10363,10 @@
         <v>7.5</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K78" s="3">
         <v>45833.0</v>
@@ -10419,7 +10398,7 @@
         <v>2.142</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I79" s="1">
         <v>2.0</v>
@@ -10610,10 +10589,10 @@
         <v>1.0</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K86" s="3">
         <v>45833.0</v>
@@ -10697,7 +10676,7 @@
         <v>0.285</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I89" s="1">
         <v>3.0</v>
@@ -10732,7 +10711,7 @@
         <v>0.2</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I90" s="1">
         <v>3.0</v>
@@ -10793,7 +10772,7 @@
         <v>6.11</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I92" s="1">
         <v>2.0</v>
@@ -10828,10 +10807,10 @@
         <v>4.16</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K93" s="3">
         <v>45833.0</v>
@@ -10889,7 +10868,7 @@
         <v>25.0</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I95" s="1">
         <v>3.0</v>
@@ -10924,10 +10903,10 @@
         <v>0.5</v>
       </c>
       <c r="H96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="K96" s="3">
         <v>45833.0</v>
@@ -11070,7 +11049,7 @@
         <v>728.0</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K104" s="3">
         <v>45840.0</v>
@@ -11311,7 +11290,7 @@
         <v>809.0</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K115" s="3">
         <v>45840.0</v>
@@ -11345,7 +11324,7 @@
         <v>784.0</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K117" s="3">
         <v>45840.0</v>
@@ -11719,7 +11698,7 @@
         <v>0.0083</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I133" s="1">
         <v>3.0</v>
@@ -12124,7 +12103,7 @@
         <v>265.0</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K151" s="3">
         <v>45840.0</v>
@@ -12388,7 +12367,7 @@
         <v>213.0</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K163" s="3">
         <v>45840.0</v>
@@ -12399,7 +12378,7 @@
         <v>483.0</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K164" s="3">
         <v>45840.0</v>
@@ -12479,7 +12458,7 @@
         <v>741.0</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K168" s="3">
         <v>45840.0</v>
@@ -12600,10 +12579,10 @@
         <v>0.2</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K173" s="3">
         <v>45840.0</v>
@@ -12632,7 +12611,7 @@
         <v>0.06875</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I174" s="1">
         <v>2.0</v>
@@ -12661,7 +12640,7 @@
         <v>9.0</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I175" s="1">
         <v>3.0</v>
@@ -12859,7 +12838,7 @@
         <v>946.0</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K184" s="3">
         <v>45840.0</v>
@@ -12870,7 +12849,7 @@
         <v>430.0</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K185" s="3">
         <v>45840.0</v>
@@ -12881,7 +12860,7 @@
         <v>649.0</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K186" s="3">
         <v>45840.0</v>
@@ -12892,7 +12871,7 @@
         <v>774.0</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K187" s="3">
         <v>45840.0</v>
@@ -12903,7 +12882,7 @@
         <v>748.0</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K188" s="3">
         <v>45840.0</v>
@@ -12952,7 +12931,7 @@
         <v>2.0</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K190" s="3">
         <v>45840.0</v>
@@ -13170,7 +13149,7 @@
         <v>815.0</v>
       </c>
       <c r="J201" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K201" s="3">
         <v>45846.0</v>
@@ -13227,7 +13206,7 @@
         <v>443.0</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K204" s="3">
         <v>45846.0</v>
@@ -13238,7 +13217,7 @@
         <v>964.0</v>
       </c>
       <c r="J205" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K205" s="3">
         <v>45846.0</v>
@@ -13318,7 +13297,7 @@
         <v>698.0</v>
       </c>
       <c r="J209" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K209" s="3">
         <v>45846.0</v>
@@ -13329,7 +13308,7 @@
         <v>270.0</v>
       </c>
       <c r="J210" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K210" s="3">
         <v>45846.0</v>
@@ -13409,7 +13388,7 @@
         <v>943.0</v>
       </c>
       <c r="J214" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K214" s="3">
         <v>45846.0</v>
@@ -13443,7 +13422,7 @@
         <v>876.0</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K216" s="3">
         <v>45846.0</v>
@@ -13495,10 +13474,10 @@
         <v>10.9</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K218" s="3">
         <v>45846.0</v>
@@ -13532,7 +13511,7 @@
         <v>679.0</v>
       </c>
       <c r="J220" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K220" s="3">
         <v>45846.0</v>
@@ -13543,7 +13522,7 @@
         <v>202.0</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K221" s="3">
         <v>45846.0</v>
@@ -13554,7 +13533,7 @@
         <v>837.0</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K222" s="3">
         <v>45846.0</v>
@@ -13634,7 +13613,7 @@
         <v>244.0</v>
       </c>
       <c r="J226" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K226" s="3">
         <v>45846.0</v>
@@ -13645,7 +13624,7 @@
         <v>225.0</v>
       </c>
       <c r="J227" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K227" s="3">
         <v>45846.0</v>
@@ -13679,7 +13658,7 @@
         <v>205.0</v>
       </c>
       <c r="J229" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K229" s="3">
         <v>45846.0</v>
@@ -13690,7 +13669,7 @@
         <v>230.0</v>
       </c>
       <c r="J230" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K230" s="3">
         <v>45846.0</v>
@@ -13747,7 +13726,7 @@
         <v>278.0</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K233" s="3">
         <v>45846.0</v>
@@ -13804,7 +13783,7 @@
         <v>840.0</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K236" s="3">
         <v>45846.0</v>
@@ -13879,10 +13858,10 @@
         <v>4.16</v>
       </c>
       <c r="H239" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K239" s="3">
         <v>45846.0</v>
@@ -13934,7 +13913,7 @@
         <v>6.25</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I241" s="1">
         <v>3.0</v>
@@ -14081,7 +14060,7 @@
         <v>6.25</v>
       </c>
       <c r="H247" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I247" s="1">
         <v>2.0</v>
@@ -14110,7 +14089,7 @@
         <v>8.0</v>
       </c>
       <c r="H248" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I248" s="1">
         <v>2.0</v>
@@ -14165,7 +14144,7 @@
         <v>4.4</v>
       </c>
       <c r="H250" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I250" s="1">
         <v>2.0</v>
@@ -14243,7 +14222,7 @@
         <v>4.54</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="K253" s="3">
         <v>45846.0</v>
@@ -14295,10 +14274,10 @@
         <v>3.07</v>
       </c>
       <c r="H255" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K255" s="3">
         <v>45846.0</v>
@@ -14324,7 +14303,7 @@
         <v>5.0</v>
       </c>
       <c r="H256" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I256" s="1">
         <v>3.0</v>
@@ -14455,7 +14434,7 @@
         <v>762.0</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K267" s="3">
         <v>45855.0</v>
@@ -14545,7 +14524,7 @@
         <v>412.0</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K273" s="3">
         <v>45855.0</v>
@@ -14556,7 +14535,7 @@
         <v>430.0</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K274" s="3">
         <v>45855.0</v>
@@ -14595,7 +14574,7 @@
         <v>248.0</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K277" s="3">
         <v>45855.0</v>
@@ -14808,7 +14787,7 @@
         <v>6.0</v>
       </c>
       <c r="J289" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K289" s="3">
         <v>45855.0</v>
@@ -15073,7 +15052,7 @@
         <v>6.0</v>
       </c>
       <c r="J305" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K305" s="8">
         <v>45860.0</v>
@@ -15122,7 +15101,7 @@
         <v>5.0</v>
       </c>
       <c r="J307" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K307" s="8">
         <v>45860.0</v>
@@ -15168,7 +15147,7 @@
         <v>0.0</v>
       </c>
       <c r="J309" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K309" s="8">
         <v>45860.0</v>
@@ -15194,7 +15173,7 @@
         <v>7.0</v>
       </c>
       <c r="J310" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K310" s="8">
         <v>45860.0</v>
@@ -15243,7 +15222,7 @@
         <v>6.0</v>
       </c>
       <c r="J312" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K312" s="8">
         <v>45860.0</v>
@@ -15269,7 +15248,7 @@
         <v>8.0</v>
       </c>
       <c r="J313" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="K313" s="8">
         <v>45860.0</v>
@@ -15346,7 +15325,7 @@
         <v>667.0</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="319">

</xml_diff>

<commit_message>
fixed dates format in excel: - or / to .
</commit_message>
<xml_diff>
--- a/data/Moser creek data.xlsx
+++ b/data/Moser creek data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="100">
   <si>
     <t>3 sites moser creek</t>
   </si>
@@ -217,6 +217,9 @@
     <t>EFN_score</t>
   </si>
   <si>
+    <t>6.25.25</t>
+  </si>
+  <si>
     <t>e no mv</t>
   </si>
   <si>
@@ -271,6 +274,9 @@
     <t>e + mv</t>
   </si>
   <si>
+    <t>7.2.25</t>
+  </si>
+  <si>
     <t>whole leaf</t>
   </si>
   <si>
@@ -280,10 +286,16 @@
     <t>dug up</t>
   </si>
   <si>
+    <t>7.8.25</t>
+  </si>
+  <si>
     <t>e w mv</t>
   </si>
   <si>
     <t>4,5</t>
+  </si>
+  <si>
+    <t>7.17.25</t>
   </si>
   <si>
     <t>NA</t>
@@ -293,6 +305,9 @@
   </si>
   <si>
     <t>DEAD top eaten</t>
+  </si>
+  <si>
+    <t>7.22.25</t>
   </si>
   <si>
     <t>DEAD</t>
@@ -305,10 +320,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m-d-yy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -340,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -348,9 +359,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -362,9 +370,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8383,8 +8388,8 @@
       <c r="F2" s="1">
         <v>4.0</v>
       </c>
-      <c r="K2" s="3">
-        <v>45833.0</v>
+      <c r="K2" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L2" s="1">
         <v>0.0</v>
@@ -8413,13 +8418,13 @@
         <v>1.875</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L3" s="1">
         <v>1.0</v>
@@ -8430,10 +8435,10 @@
         <v>728.0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="3">
-        <v>45833.0</v>
+        <v>69</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -8455,8 +8460,8 @@
       <c r="F5" s="1">
         <v>6.0</v>
       </c>
-      <c r="K5" s="3">
-        <v>45833.0</v>
+      <c r="K5" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L5" s="1">
         <v>0.0</v>
@@ -8481,8 +8486,8 @@
       <c r="F6" s="1">
         <v>3.0</v>
       </c>
-      <c r="K6" s="3">
-        <v>45833.0</v>
+      <c r="K6" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L6" s="1">
         <v>0.0</v>
@@ -8507,8 +8512,8 @@
       <c r="F7" s="1">
         <v>8.0</v>
       </c>
-      <c r="K7" s="3">
-        <v>45833.0</v>
+      <c r="K7" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L7" s="1">
         <v>1.0</v>
@@ -8533,8 +8538,8 @@
       <c r="F8" s="1">
         <v>1.0</v>
       </c>
-      <c r="K8" s="3">
-        <v>45833.0</v>
+      <c r="K8" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L8" s="1">
         <v>0.0</v>
@@ -8563,13 +8568,13 @@
         <v>0.625</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L9" s="1">
         <v>1.0</v>
@@ -8594,8 +8599,8 @@
       <c r="F10" s="1">
         <v>5.0</v>
       </c>
-      <c r="K10" s="3">
-        <v>45833.0</v>
+      <c r="K10" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L10" s="1">
         <v>1.0</v>
@@ -8620,8 +8625,8 @@
       <c r="F11" s="1">
         <v>6.0</v>
       </c>
-      <c r="K11" s="3">
-        <v>45833.0</v>
+      <c r="K11" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L11" s="1">
         <v>0.0</v>
@@ -8646,8 +8651,8 @@
       <c r="F12" s="1">
         <v>8.0</v>
       </c>
-      <c r="K12" s="3">
-        <v>45833.0</v>
+      <c r="K12" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L12" s="1">
         <v>1.0</v>
@@ -8672,8 +8677,8 @@
       <c r="F13" s="1">
         <v>0.0</v>
       </c>
-      <c r="K13" s="3">
-        <v>45833.0</v>
+      <c r="K13" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L13" s="1">
         <v>1.0</v>
@@ -8699,10 +8704,10 @@
         <v>4.0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="3">
-        <v>45833.0</v>
+        <v>70</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L14" s="1">
         <v>0.0</v>
@@ -8727,8 +8732,8 @@
       <c r="F15" s="1">
         <v>4.0</v>
       </c>
-      <c r="K15" s="3">
-        <v>45833.0</v>
+      <c r="K15" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L15" s="1">
         <v>1.0</v>
@@ -8753,8 +8758,8 @@
       <c r="F16" s="1">
         <v>6.0</v>
       </c>
-      <c r="K16" s="3">
-        <v>45833.0</v>
+      <c r="K16" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L16" s="1">
         <v>0.0</v>
@@ -8765,10 +8770,10 @@
         <v>809.0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" s="3">
-        <v>45833.0</v>
+        <v>71</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18">
@@ -8776,10 +8781,10 @@
         <v>784.0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K18" s="3">
-        <v>45833.0</v>
+        <v>71</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19">
@@ -8801,8 +8806,8 @@
       <c r="F19" s="1">
         <v>1.0</v>
       </c>
-      <c r="K19" s="3">
-        <v>45833.0</v>
+      <c r="K19" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L19" s="1">
         <v>0.0</v>
@@ -8827,8 +8832,8 @@
       <c r="F20" s="1">
         <v>4.0</v>
       </c>
-      <c r="K20" s="3">
-        <v>45833.0</v>
+      <c r="K20" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L20" s="1">
         <v>0.0</v>
@@ -8853,8 +8858,8 @@
       <c r="F21" s="1">
         <v>7.0</v>
       </c>
-      <c r="K21" s="3">
-        <v>45833.0</v>
+      <c r="K21" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L21" s="1">
         <v>1.0</v>
@@ -8880,10 +8885,10 @@
         <v>5.0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="3">
-        <v>45833.0</v>
+        <v>70</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L22" s="1">
         <v>0.0</v>
@@ -8894,10 +8899,10 @@
         <v>830.0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" s="3">
-        <v>45833.0</v>
+        <v>71</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24">
@@ -8919,8 +8924,8 @@
       <c r="F24" s="1">
         <v>2.0</v>
       </c>
-      <c r="K24" s="3">
-        <v>45833.0</v>
+      <c r="K24" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L24" s="1">
         <v>0.0</v>
@@ -8945,8 +8950,8 @@
       <c r="F25" s="1">
         <v>6.0</v>
       </c>
-      <c r="K25" s="3">
-        <v>45833.0</v>
+      <c r="K25" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L25" s="1">
         <v>0.0</v>
@@ -8971,8 +8976,8 @@
       <c r="F26" s="1">
         <v>3.0</v>
       </c>
-      <c r="K26" s="3">
-        <v>45833.0</v>
+      <c r="K26" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L26" s="1">
         <v>0.0</v>
@@ -8997,8 +9002,8 @@
       <c r="F27" s="1">
         <v>6.0</v>
       </c>
-      <c r="K27" s="3">
-        <v>45833.0</v>
+      <c r="K27" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L27" s="1">
         <v>1.0</v>
@@ -9023,8 +9028,8 @@
       <c r="F28" s="1">
         <v>4.0</v>
       </c>
-      <c r="K28" s="3">
-        <v>45833.0</v>
+      <c r="K28" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L28" s="1">
         <v>0.0</v>
@@ -9049,8 +9054,8 @@
       <c r="F29" s="1">
         <v>6.0</v>
       </c>
-      <c r="K29" s="3">
-        <v>45833.0</v>
+      <c r="K29" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L29" s="1">
         <v>0.0</v>
@@ -9075,8 +9080,8 @@
       <c r="F30" s="1">
         <v>6.0</v>
       </c>
-      <c r="K30" s="3">
-        <v>45833.0</v>
+      <c r="K30" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L30" s="1">
         <v>0.0</v>
@@ -9101,8 +9106,8 @@
       <c r="F31" s="1">
         <v>4.0</v>
       </c>
-      <c r="K31" s="3">
-        <v>45833.0</v>
+      <c r="K31" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L31" s="1">
         <v>0.0</v>
@@ -9127,8 +9132,8 @@
       <c r="F32" s="1">
         <v>6.0</v>
       </c>
-      <c r="K32" s="3">
-        <v>45833.0</v>
+      <c r="K32" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L32" s="1">
         <v>0.0</v>
@@ -9153,8 +9158,8 @@
       <c r="F33" s="1">
         <v>2.0</v>
       </c>
-      <c r="K33" s="3">
-        <v>45833.0</v>
+      <c r="K33" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L33" s="1">
         <v>0.0</v>
@@ -9179,8 +9184,8 @@
       <c r="F34" s="1">
         <v>4.0</v>
       </c>
-      <c r="K34" s="3">
-        <v>45833.0</v>
+      <c r="K34" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L34" s="1">
         <v>0.0</v>
@@ -9205,8 +9210,8 @@
       <c r="F35" s="1">
         <v>0.0</v>
       </c>
-      <c r="K35" s="3">
-        <v>45833.0</v>
+      <c r="K35" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L35" s="1">
         <v>0.0</v>
@@ -9231,8 +9236,8 @@
       <c r="F36" s="1">
         <v>2.0</v>
       </c>
-      <c r="K36" s="3">
-        <v>45833.0</v>
+      <c r="K36" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L36" s="1">
         <v>0.0</v>
@@ -9257,8 +9262,8 @@
       <c r="F37" s="1">
         <v>4.0</v>
       </c>
-      <c r="K37" s="3">
-        <v>45833.0</v>
+      <c r="K37" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L37" s="1">
         <v>0.0</v>
@@ -9287,13 +9292,13 @@
         <v>0.2</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I38" s="1">
         <v>3.0</v>
       </c>
-      <c r="K38" s="3">
-        <v>45833.0</v>
+      <c r="K38" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L38" s="1">
         <v>2.0</v>
@@ -9318,8 +9323,8 @@
       <c r="F39" s="1">
         <v>8.0</v>
       </c>
-      <c r="K39" s="3">
-        <v>45833.0</v>
+      <c r="K39" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L39" s="1">
         <v>0.0</v>
@@ -9344,8 +9349,8 @@
       <c r="F40" s="1">
         <v>5.0</v>
       </c>
-      <c r="K40" s="3">
-        <v>45833.0</v>
+      <c r="K40" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L40" s="1">
         <v>0.0</v>
@@ -9370,8 +9375,8 @@
       <c r="F41" s="1">
         <v>5.0</v>
       </c>
-      <c r="K41" s="3">
-        <v>45833.0</v>
+      <c r="K41" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L41" s="1">
         <v>0.0</v>
@@ -9396,8 +9401,8 @@
       <c r="F42" s="1">
         <v>4.0</v>
       </c>
-      <c r="K42" s="3">
-        <v>45833.0</v>
+      <c r="K42" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L42" s="1">
         <v>0.0</v>
@@ -9422,8 +9427,8 @@
       <c r="F43" s="1">
         <v>4.0</v>
       </c>
-      <c r="K43" s="3">
-        <v>45833.0</v>
+      <c r="K43" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L43" s="1">
         <v>1.0</v>
@@ -9448,8 +9453,8 @@
       <c r="F44" s="1">
         <v>10.0</v>
       </c>
-      <c r="K44" s="3">
-        <v>45833.0</v>
+      <c r="K44" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L44" s="1">
         <v>2.0</v>
@@ -9474,8 +9479,8 @@
       <c r="F45" s="1">
         <v>1.0</v>
       </c>
-      <c r="K45" s="3">
-        <v>45833.0</v>
+      <c r="K45" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L45" s="1">
         <v>0.0</v>
@@ -9504,13 +9509,13 @@
         <v>0.5</v>
       </c>
       <c r="H46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I46" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="K46" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L46" s="1">
         <v>1.0</v>
@@ -9539,13 +9544,13 @@
         <v>1.583</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K47" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L47" s="1">
         <v>1.0</v>
@@ -9574,13 +9579,13 @@
         <v>0.83</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I48" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I48" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="K48" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L48" s="1">
         <v>1.0</v>
@@ -9605,8 +9610,8 @@
       <c r="F49" s="1">
         <v>6.0</v>
       </c>
-      <c r="K49" s="3">
-        <v>45833.0</v>
+      <c r="K49" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L49" s="1">
         <v>0.0</v>
@@ -9631,8 +9636,8 @@
       <c r="F50" s="1">
         <v>10.0</v>
       </c>
-      <c r="K50" s="3">
-        <v>45833.0</v>
+      <c r="K50" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L50" s="1">
         <v>0.0</v>
@@ -9657,8 +9662,8 @@
       <c r="F51" s="1">
         <v>5.0</v>
       </c>
-      <c r="K51" s="3">
-        <v>45833.0</v>
+      <c r="K51" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L51" s="1">
         <v>1.0</v>
@@ -9683,8 +9688,8 @@
       <c r="F52" s="1">
         <v>6.0</v>
       </c>
-      <c r="K52" s="3">
-        <v>45833.0</v>
+      <c r="K52" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L52" s="1">
         <v>0.0</v>
@@ -9709,8 +9714,8 @@
       <c r="F53" s="1">
         <v>12.0</v>
       </c>
-      <c r="K53" s="3">
-        <v>45833.0</v>
+      <c r="K53" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L53" s="1">
         <v>1.0</v>
@@ -9735,8 +9740,8 @@
       <c r="F54" s="1">
         <v>0.0</v>
       </c>
-      <c r="K54" s="3">
-        <v>45833.0</v>
+      <c r="K54" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L54" s="1">
         <v>0.0</v>
@@ -9761,8 +9766,8 @@
       <c r="F55" s="1">
         <v>9.0</v>
       </c>
-      <c r="K55" s="3">
-        <v>45833.0</v>
+      <c r="K55" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L55" s="1">
         <v>1.0</v>
@@ -9787,8 +9792,8 @@
       <c r="F56" s="1">
         <v>13.0</v>
       </c>
-      <c r="K56" s="3">
-        <v>45833.0</v>
+      <c r="K56" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L56" s="1">
         <v>1.0</v>
@@ -9813,8 +9818,8 @@
       <c r="F57" s="1">
         <v>9.0</v>
       </c>
-      <c r="K57" s="3">
-        <v>45833.0</v>
+      <c r="K57" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L57" s="1">
         <v>1.0</v>
@@ -9839,8 +9844,8 @@
       <c r="F58" s="1">
         <v>11.0</v>
       </c>
-      <c r="K58" s="3">
-        <v>45833.0</v>
+      <c r="K58" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L58" s="1">
         <v>1.0</v>
@@ -9865,8 +9870,8 @@
       <c r="F59" s="1">
         <v>8.0</v>
       </c>
-      <c r="K59" s="3">
-        <v>45833.0</v>
+      <c r="K59" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L59" s="1">
         <v>0.0</v>
@@ -9891,8 +9896,8 @@
       <c r="F60" s="1">
         <v>9.0</v>
       </c>
-      <c r="K60" s="3">
-        <v>45833.0</v>
+      <c r="K60" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L60" s="1">
         <v>1.0</v>
@@ -9917,8 +9922,8 @@
       <c r="F61" s="1">
         <v>5.0</v>
       </c>
-      <c r="K61" s="3">
-        <v>45833.0</v>
+      <c r="K61" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L61" s="1">
         <v>1.0</v>
@@ -9943,8 +9948,8 @@
       <c r="F62" s="1">
         <v>7.0</v>
       </c>
-      <c r="K62" s="3">
-        <v>45833.0</v>
+      <c r="K62" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L62" s="1">
         <v>1.0</v>
@@ -9969,8 +9974,8 @@
       <c r="F63" s="1">
         <v>4.0</v>
       </c>
-      <c r="K63" s="3">
-        <v>45833.0</v>
+      <c r="K63" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L63" s="1">
         <v>0.0</v>
@@ -9995,8 +10000,8 @@
       <c r="F64" s="1">
         <v>5.0</v>
       </c>
-      <c r="K64" s="3">
-        <v>45833.0</v>
+      <c r="K64" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L64" s="1">
         <v>0.0</v>
@@ -10021,8 +10026,8 @@
       <c r="F65" s="1">
         <v>10.0</v>
       </c>
-      <c r="K65" s="3">
-        <v>45833.0</v>
+      <c r="K65" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L65" s="1">
         <v>1.0</v>
@@ -10050,8 +10055,8 @@
       <c r="J66" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K66" s="3">
-        <v>45833.0</v>
+      <c r="K66" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L66" s="1">
         <v>0.0</v>
@@ -10076,8 +10081,8 @@
       <c r="F67" s="1">
         <v>6.0</v>
       </c>
-      <c r="K67" s="3">
-        <v>45833.0</v>
+      <c r="K67" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L67" s="1">
         <v>0.0</v>
@@ -10102,8 +10107,8 @@
       <c r="F68" s="1">
         <v>6.0</v>
       </c>
-      <c r="K68" s="3">
-        <v>45833.0</v>
+      <c r="K68" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L68" s="1">
         <v>1.0</v>
@@ -10129,10 +10134,10 @@
         <v>6.0</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K69" s="3">
-        <v>45833.0</v>
+        <v>74</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L69" s="1">
         <v>0.0</v>
@@ -10161,13 +10166,13 @@
         <v>0.875</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K70" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K70" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L70" s="1">
         <v>1.0</v>
@@ -10192,8 +10197,8 @@
       <c r="F71" s="1">
         <v>2.0</v>
       </c>
-      <c r="K71" s="3">
-        <v>45833.0</v>
+      <c r="K71" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L71" s="1">
         <v>0.0</v>
@@ -10218,8 +10223,8 @@
       <c r="F72" s="1">
         <v>7.0</v>
       </c>
-      <c r="K72" s="3">
-        <v>45833.0</v>
+      <c r="K72" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L72" s="1">
         <v>0.0</v>
@@ -10244,8 +10249,8 @@
       <c r="F73" s="1">
         <v>9.0</v>
       </c>
-      <c r="K73" s="3">
-        <v>45833.0</v>
+      <c r="K73" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L73" s="1">
         <v>1.0</v>
@@ -10270,8 +10275,8 @@
       <c r="F74" s="1">
         <v>8.0</v>
       </c>
-      <c r="K74" s="3">
-        <v>45833.0</v>
+      <c r="K74" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L74" s="1">
         <v>1.0</v>
@@ -10296,8 +10301,8 @@
       <c r="F75" s="1">
         <v>11.0</v>
       </c>
-      <c r="K75" s="3">
-        <v>45833.0</v>
+      <c r="K75" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L75" s="1">
         <v>1.0</v>
@@ -10308,10 +10313,10 @@
         <v>622.0</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K76" s="3">
-        <v>45833.0</v>
+        <v>76</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="77">
@@ -10333,8 +10338,8 @@
       <c r="F77" s="1">
         <v>14.0</v>
       </c>
-      <c r="K77" s="3">
-        <v>45833.0</v>
+      <c r="K77" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L77" s="1">
         <v>2.0</v>
@@ -10363,13 +10368,13 @@
         <v>7.5</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K78" s="3">
-        <v>45833.0</v>
+        <v>78</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L78" s="1">
         <v>1.0</v>
@@ -10398,13 +10403,13 @@
         <v>2.142</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I79" s="1">
         <v>2.0</v>
       </c>
-      <c r="K79" s="3">
-        <v>45833.0</v>
+      <c r="K79" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L79" s="1">
         <v>1.0</v>
@@ -10429,8 +10434,8 @@
       <c r="F80" s="1">
         <v>5.0</v>
       </c>
-      <c r="K80" s="3">
-        <v>45833.0</v>
+      <c r="K80" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L80" s="1">
         <v>0.0</v>
@@ -10455,8 +10460,8 @@
       <c r="F81" s="1">
         <v>0.0</v>
       </c>
-      <c r="K81" s="3">
-        <v>45833.0</v>
+      <c r="K81" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L81" s="1">
         <v>0.0</v>
@@ -10481,8 +10486,8 @@
       <c r="F82" s="1">
         <v>6.0</v>
       </c>
-      <c r="K82" s="3">
-        <v>45833.0</v>
+      <c r="K82" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L82" s="1">
         <v>1.0</v>
@@ -10507,8 +10512,8 @@
       <c r="F83" s="1">
         <v>0.0</v>
       </c>
-      <c r="K83" s="3">
-        <v>45833.0</v>
+      <c r="K83" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L83" s="1">
         <v>0.0</v>
@@ -10533,8 +10538,8 @@
       <c r="F84" s="1">
         <v>9.0</v>
       </c>
-      <c r="K84" s="3">
-        <v>45833.0</v>
+      <c r="K84" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L84" s="1">
         <v>1.0</v>
@@ -10559,8 +10564,8 @@
       <c r="F85" s="1">
         <v>11.0</v>
       </c>
-      <c r="K85" s="3">
-        <v>45833.0</v>
+      <c r="K85" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L85" s="1">
         <v>2.0</v>
@@ -10589,13 +10594,13 @@
         <v>1.0</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K86" s="3">
-        <v>45833.0</v>
+        <v>81</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L86" s="1">
         <v>2.0</v>
@@ -10620,8 +10625,8 @@
       <c r="F87" s="1">
         <v>8.0</v>
       </c>
-      <c r="K87" s="3">
-        <v>45833.0</v>
+      <c r="K87" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L87" s="1">
         <v>1.0</v>
@@ -10646,8 +10651,8 @@
       <c r="F88" s="1">
         <v>5.0</v>
       </c>
-      <c r="K88" s="3">
-        <v>45833.0</v>
+      <c r="K88" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L88" s="1">
         <v>0.0</v>
@@ -10676,13 +10681,13 @@
         <v>0.285</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I89" s="1">
         <v>3.0</v>
       </c>
-      <c r="K89" s="3">
-        <v>45833.0</v>
+      <c r="K89" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L89" s="1">
         <v>0.0</v>
@@ -10711,13 +10716,13 @@
         <v>0.2</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I90" s="1">
         <v>3.0</v>
       </c>
-      <c r="K90" s="3">
-        <v>45833.0</v>
+      <c r="K90" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L90" s="1">
         <v>2.0</v>
@@ -10742,8 +10747,8 @@
       <c r="F91" s="1">
         <v>4.0</v>
       </c>
-      <c r="K91" s="3">
-        <v>45833.0</v>
+      <c r="K91" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L91" s="1">
         <v>0.0</v>
@@ -10772,13 +10777,13 @@
         <v>6.11</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I92" s="1">
         <v>2.0</v>
       </c>
-      <c r="K92" s="3">
-        <v>45833.0</v>
+      <c r="K92" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L92" s="1">
         <v>1.0</v>
@@ -10807,13 +10812,13 @@
         <v>4.16</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K93" s="3">
-        <v>45833.0</v>
+        <v>84</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L93" s="1">
         <v>2.0</v>
@@ -10838,8 +10843,8 @@
       <c r="F94" s="1">
         <v>5.0</v>
       </c>
-      <c r="K94" s="3">
-        <v>45833.0</v>
+      <c r="K94" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L94" s="1">
         <v>1.0</v>
@@ -10868,13 +10873,13 @@
         <v>25.0</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I95" s="1">
         <v>3.0</v>
       </c>
-      <c r="K95" s="3">
-        <v>45833.0</v>
+      <c r="K95" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L95" s="1">
         <v>2.0</v>
@@ -10903,13 +10908,13 @@
         <v>0.5</v>
       </c>
       <c r="H96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K96" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K96" s="3">
-        <v>45833.0</v>
       </c>
       <c r="L96" s="1">
         <v>2.0</v>
@@ -10919,8 +10924,8 @@
       <c r="A97" s="1">
         <v>443.0</v>
       </c>
-      <c r="K97" s="3">
-        <v>45833.0</v>
+      <c r="K97" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="98">
@@ -10942,8 +10947,8 @@
       <c r="F98" s="1">
         <v>6.0</v>
       </c>
-      <c r="K98" s="3">
-        <v>45833.0</v>
+      <c r="K98" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L98" s="1">
         <v>0.0</v>
@@ -10968,8 +10973,8 @@
       <c r="F99" s="1">
         <v>7.0</v>
       </c>
-      <c r="K99" s="3">
-        <v>45833.0</v>
+      <c r="K99" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L99" s="1">
         <v>1.0</v>
@@ -10994,8 +10999,8 @@
       <c r="F101" s="1">
         <v>3.0</v>
       </c>
-      <c r="K101" s="3">
-        <v>45840.0</v>
+      <c r="K101" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="102">
@@ -11017,8 +11022,8 @@
       <c r="F102" s="1">
         <v>3.0</v>
       </c>
-      <c r="K102" s="3">
-        <v>45840.0</v>
+      <c r="K102" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="103">
@@ -11040,8 +11045,8 @@
       <c r="F103" s="1">
         <v>7.0</v>
       </c>
-      <c r="K103" s="3">
-        <v>45840.0</v>
+      <c r="K103" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="104">
@@ -11051,8 +11056,8 @@
       <c r="J104" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K104" s="3">
-        <v>45840.0</v>
+      <c r="K104" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="105">
@@ -11074,8 +11079,8 @@
       <c r="F105" s="1">
         <v>7.0</v>
       </c>
-      <c r="K105" s="3">
-        <v>45840.0</v>
+      <c r="K105" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="106">
@@ -11097,8 +11102,8 @@
       <c r="F106" s="1">
         <v>5.0</v>
       </c>
-      <c r="K106" s="3">
-        <v>45840.0</v>
+      <c r="K106" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="107">
@@ -11120,8 +11125,8 @@
       <c r="F107" s="1">
         <v>3.0</v>
       </c>
-      <c r="K107" s="3">
-        <v>45840.0</v>
+      <c r="K107" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="108">
@@ -11143,8 +11148,8 @@
       <c r="F108" s="1">
         <v>0.0</v>
       </c>
-      <c r="K108" s="3">
-        <v>45840.0</v>
+      <c r="K108" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="109">
@@ -11166,8 +11171,8 @@
       <c r="F109" s="1">
         <v>4.0</v>
       </c>
-      <c r="K109" s="3">
-        <v>45840.0</v>
+      <c r="K109" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="110">
@@ -11189,8 +11194,8 @@
       <c r="F110" s="1">
         <v>4.0</v>
       </c>
-      <c r="K110" s="3">
-        <v>45840.0</v>
+      <c r="K110" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="111">
@@ -11212,8 +11217,8 @@
       <c r="F111" s="1">
         <v>9.0</v>
       </c>
-      <c r="K111" s="3">
-        <v>45840.0</v>
+      <c r="K111" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="112">
@@ -11235,8 +11240,8 @@
       <c r="F112" s="1">
         <v>0.0</v>
       </c>
-      <c r="K112" s="3">
-        <v>45840.0</v>
+      <c r="K112" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="113">
@@ -11258,8 +11263,8 @@
       <c r="F113" s="1">
         <v>3.0</v>
       </c>
-      <c r="K113" s="3">
-        <v>45840.0</v>
+      <c r="K113" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="114">
@@ -11281,8 +11286,8 @@
       <c r="F114" s="1">
         <v>6.0</v>
       </c>
-      <c r="K114" s="3">
-        <v>45840.0</v>
+      <c r="K114" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="115">
@@ -11292,8 +11297,8 @@
       <c r="J115" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K115" s="3">
-        <v>45840.0</v>
+      <c r="K115" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="116">
@@ -11315,8 +11320,8 @@
       <c r="F116" s="1">
         <v>1.0</v>
       </c>
-      <c r="K116" s="3">
-        <v>45840.0</v>
+      <c r="K116" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="117">
@@ -11326,8 +11331,8 @@
       <c r="J117" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K117" s="3">
-        <v>45840.0</v>
+      <c r="K117" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="118">
@@ -11349,8 +11354,8 @@
       <c r="F118" s="1">
         <v>1.0</v>
       </c>
-      <c r="K118" s="3">
-        <v>45840.0</v>
+      <c r="K118" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="119">
@@ -11372,8 +11377,8 @@
       <c r="F119" s="1">
         <v>4.0</v>
       </c>
-      <c r="K119" s="3">
-        <v>45840.0</v>
+      <c r="K119" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="120">
@@ -11395,8 +11400,8 @@
       <c r="F120" s="1">
         <v>8.0</v>
       </c>
-      <c r="K120" s="3">
-        <v>45840.0</v>
+      <c r="K120" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="121">
@@ -11418,8 +11423,8 @@
       <c r="F121" s="1">
         <v>4.0</v>
       </c>
-      <c r="K121" s="3">
-        <v>45840.0</v>
+      <c r="K121" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="122">
@@ -11441,8 +11446,8 @@
       <c r="F122" s="1">
         <v>2.0</v>
       </c>
-      <c r="K122" s="3">
-        <v>45840.0</v>
+      <c r="K122" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="123">
@@ -11464,8 +11469,8 @@
       <c r="F123" s="1">
         <v>3.0</v>
       </c>
-      <c r="K123" s="3">
-        <v>45840.0</v>
+      <c r="K123" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="124">
@@ -11487,8 +11492,8 @@
       <c r="F124" s="1">
         <v>2.0</v>
       </c>
-      <c r="K124" s="3">
-        <v>45840.0</v>
+      <c r="K124" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="125">
@@ -11510,8 +11515,8 @@
       <c r="F125" s="1">
         <v>3.0</v>
       </c>
-      <c r="K125" s="3">
-        <v>45840.0</v>
+      <c r="K125" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="126">
@@ -11533,8 +11538,8 @@
       <c r="F126" s="1">
         <v>4.0</v>
       </c>
-      <c r="K126" s="3">
-        <v>45840.0</v>
+      <c r="K126" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="127">
@@ -11556,8 +11561,8 @@
       <c r="F127" s="1">
         <v>0.0</v>
       </c>
-      <c r="K127" s="3">
-        <v>45840.0</v>
+      <c r="K127" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="128">
@@ -11579,8 +11584,8 @@
       <c r="F128" s="1">
         <v>4.0</v>
       </c>
-      <c r="K128" s="3">
-        <v>45840.0</v>
+      <c r="K128" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="129">
@@ -11602,8 +11607,8 @@
       <c r="F129" s="1">
         <v>0.0</v>
       </c>
-      <c r="K129" s="3">
-        <v>45840.0</v>
+      <c r="K129" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="130">
@@ -11625,8 +11630,8 @@
       <c r="F130" s="1">
         <v>6.0</v>
       </c>
-      <c r="K130" s="3">
-        <v>45840.0</v>
+      <c r="K130" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="131">
@@ -11648,8 +11653,8 @@
       <c r="F131" s="1">
         <v>6.0</v>
       </c>
-      <c r="K131" s="3">
-        <v>45840.0</v>
+      <c r="K131" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="132">
@@ -11671,8 +11676,8 @@
       <c r="F132" s="1">
         <v>9.0</v>
       </c>
-      <c r="K132" s="3">
-        <v>45840.0</v>
+      <c r="K132" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="133">
@@ -11694,17 +11699,17 @@
       <c r="F133" s="1">
         <v>6.0</v>
       </c>
-      <c r="G133" s="4">
+      <c r="G133" s="3">
         <v>0.0083</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I133" s="1">
         <v>3.0</v>
       </c>
-      <c r="K133" s="3">
-        <v>45840.0</v>
+      <c r="K133" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="134">
@@ -11726,8 +11731,8 @@
       <c r="F134" s="1">
         <v>0.0</v>
       </c>
-      <c r="K134" s="3">
-        <v>45840.0</v>
+      <c r="K134" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="135">
@@ -11749,8 +11754,8 @@
       <c r="F135" s="1">
         <v>0.0</v>
       </c>
-      <c r="K135" s="3">
-        <v>45840.0</v>
+      <c r="K135" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="136">
@@ -11772,8 +11777,8 @@
       <c r="F136" s="1">
         <v>8.0</v>
       </c>
-      <c r="K136" s="3">
-        <v>45840.0</v>
+      <c r="K136" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="137">
@@ -11795,8 +11800,8 @@
       <c r="F137" s="1">
         <v>0.0</v>
       </c>
-      <c r="K137" s="3">
-        <v>45840.0</v>
+      <c r="K137" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="138">
@@ -11818,8 +11823,8 @@
       <c r="F138" s="1">
         <v>6.0</v>
       </c>
-      <c r="K138" s="3">
-        <v>45840.0</v>
+      <c r="K138" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="139">
@@ -11841,8 +11846,8 @@
       <c r="F139" s="1">
         <v>6.0</v>
       </c>
-      <c r="K139" s="3">
-        <v>45840.0</v>
+      <c r="K139" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="140">
@@ -11864,8 +11869,8 @@
       <c r="F140" s="1">
         <v>8.0</v>
       </c>
-      <c r="K140" s="3">
-        <v>45840.0</v>
+      <c r="K140" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="141">
@@ -11887,8 +11892,8 @@
       <c r="F141" s="1">
         <v>7.0</v>
       </c>
-      <c r="K141" s="3">
-        <v>45840.0</v>
+      <c r="K141" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="142">
@@ -11910,8 +11915,8 @@
       <c r="F142" s="1">
         <v>0.0</v>
       </c>
-      <c r="K142" s="3">
-        <v>45840.0</v>
+      <c r="K142" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="143">
@@ -11933,8 +11938,8 @@
       <c r="F143" s="1">
         <v>12.0</v>
       </c>
-      <c r="K143" s="3">
-        <v>45840.0</v>
+      <c r="K143" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="144">
@@ -11956,8 +11961,8 @@
       <c r="F144" s="1">
         <v>4.0</v>
       </c>
-      <c r="K144" s="3">
-        <v>45840.0</v>
+      <c r="K144" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="145">
@@ -11979,8 +11984,8 @@
       <c r="F145" s="1">
         <v>4.0</v>
       </c>
-      <c r="K145" s="3">
-        <v>45840.0</v>
+      <c r="K145" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="146">
@@ -12002,8 +12007,8 @@
       <c r="F146" s="1">
         <v>9.0</v>
       </c>
-      <c r="K146" s="3">
-        <v>45840.0</v>
+      <c r="K146" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="147">
@@ -12025,8 +12030,8 @@
       <c r="F147" s="1">
         <v>6.0</v>
       </c>
-      <c r="K147" s="3">
-        <v>45840.0</v>
+      <c r="K147" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="148">
@@ -12048,8 +12053,8 @@
       <c r="F148" s="1">
         <v>4.0</v>
       </c>
-      <c r="K148" s="3">
-        <v>45840.0</v>
+      <c r="K148" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="149">
@@ -12071,8 +12076,8 @@
       <c r="F149" s="1">
         <v>9.0</v>
       </c>
-      <c r="K149" s="3">
-        <v>45840.0</v>
+      <c r="K149" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="150">
@@ -12094,8 +12099,8 @@
       <c r="F150" s="1">
         <v>4.0</v>
       </c>
-      <c r="K150" s="3">
-        <v>45840.0</v>
+      <c r="K150" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="151">
@@ -12105,8 +12110,8 @@
       <c r="J151" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K151" s="3">
-        <v>45840.0</v>
+      <c r="K151" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="152">
@@ -12128,8 +12133,8 @@
       <c r="F152" s="1">
         <v>9.0</v>
       </c>
-      <c r="K152" s="3">
-        <v>45840.0</v>
+      <c r="K152" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="153">
@@ -12151,8 +12156,8 @@
       <c r="F153" s="1">
         <v>6.0</v>
       </c>
-      <c r="K153" s="3">
-        <v>45840.0</v>
+      <c r="K153" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="154">
@@ -12174,8 +12179,8 @@
       <c r="F154" s="1">
         <v>6.0</v>
       </c>
-      <c r="K154" s="3">
-        <v>45840.0</v>
+      <c r="K154" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="155">
@@ -12197,8 +12202,8 @@
       <c r="F155" s="1">
         <v>4.0</v>
       </c>
-      <c r="K155" s="3">
-        <v>45840.0</v>
+      <c r="K155" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="156">
@@ -12220,8 +12225,8 @@
       <c r="F156" s="1">
         <v>4.0</v>
       </c>
-      <c r="K156" s="3">
-        <v>45840.0</v>
+      <c r="K156" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="157">
@@ -12243,8 +12248,8 @@
       <c r="F157" s="1">
         <v>4.0</v>
       </c>
-      <c r="K157" s="3">
-        <v>45840.0</v>
+      <c r="K157" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="158">
@@ -12266,8 +12271,8 @@
       <c r="F158" s="1">
         <v>8.0</v>
       </c>
-      <c r="K158" s="3">
-        <v>45840.0</v>
+      <c r="K158" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="159">
@@ -12289,8 +12294,8 @@
       <c r="F159" s="1">
         <v>6.0</v>
       </c>
-      <c r="K159" s="3">
-        <v>45840.0</v>
+      <c r="K159" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="160">
@@ -12312,8 +12317,8 @@
       <c r="F160" s="1">
         <v>3.0</v>
       </c>
-      <c r="K160" s="3">
-        <v>45840.0</v>
+      <c r="K160" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="161">
@@ -12335,8 +12340,8 @@
       <c r="F161" s="1">
         <v>6.0</v>
       </c>
-      <c r="K161" s="3">
-        <v>45840.0</v>
+      <c r="K161" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="162">
@@ -12358,8 +12363,8 @@
       <c r="F162" s="1">
         <v>9.0</v>
       </c>
-      <c r="K162" s="3">
-        <v>45840.0</v>
+      <c r="K162" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="163">
@@ -12369,8 +12374,8 @@
       <c r="J163" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K163" s="3">
-        <v>45840.0</v>
+      <c r="K163" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="164">
@@ -12380,8 +12385,8 @@
       <c r="J164" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K164" s="3">
-        <v>45840.0</v>
+      <c r="K164" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="165">
@@ -12403,8 +12408,8 @@
       <c r="F165" s="1">
         <v>1.0</v>
       </c>
-      <c r="K165" s="3">
-        <v>45840.0</v>
+      <c r="K165" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="166">
@@ -12426,8 +12431,8 @@
       <c r="F166" s="1">
         <v>11.0</v>
       </c>
-      <c r="K166" s="3">
-        <v>45840.0</v>
+      <c r="K166" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="167">
@@ -12449,8 +12454,8 @@
       <c r="F167" s="1">
         <v>9.0</v>
       </c>
-      <c r="K167" s="3">
-        <v>45840.0</v>
+      <c r="K167" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="168">
@@ -12460,8 +12465,8 @@
       <c r="J168" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K168" s="3">
-        <v>45840.0</v>
+      <c r="K168" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="169">
@@ -12483,8 +12488,8 @@
       <c r="F169" s="1">
         <v>12.0</v>
       </c>
-      <c r="K169" s="3">
-        <v>45840.0</v>
+      <c r="K169" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="170">
@@ -12506,8 +12511,8 @@
       <c r="F170" s="1">
         <v>6.0</v>
       </c>
-      <c r="K170" s="3">
-        <v>45840.0</v>
+      <c r="K170" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="171">
@@ -12529,8 +12534,8 @@
       <c r="F171" s="1">
         <v>9.0</v>
       </c>
-      <c r="K171" s="3">
-        <v>45840.0</v>
+      <c r="K171" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="172">
@@ -12552,8 +12557,8 @@
       <c r="F172" s="1">
         <v>0.0</v>
       </c>
-      <c r="K172" s="3">
-        <v>45840.0</v>
+      <c r="K172" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="173">
@@ -12575,17 +12580,17 @@
       <c r="F173" s="1">
         <v>5.0</v>
       </c>
-      <c r="G173" s="5">
+      <c r="G173" s="4">
         <v>0.2</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K173" s="3">
-        <v>45840.0</v>
+        <v>75</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="174">
@@ -12607,17 +12612,17 @@
       <c r="F174" s="1">
         <v>8.0</v>
       </c>
-      <c r="G174" s="4">
+      <c r="G174" s="3">
         <v>0.06875</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I174" s="1">
         <v>2.0</v>
       </c>
-      <c r="K174" s="3">
-        <v>45840.0</v>
+      <c r="K174" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="175">
@@ -12640,13 +12645,13 @@
         <v>9.0</v>
       </c>
       <c r="H175" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I175" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="K175" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="I175" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="K175" s="3">
-        <v>45840.0</v>
       </c>
     </row>
     <row r="176">
@@ -12668,8 +12673,8 @@
       <c r="F176" s="1">
         <v>8.0</v>
       </c>
-      <c r="K176" s="3">
-        <v>45840.0</v>
+      <c r="K176" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="177">
@@ -12691,8 +12696,8 @@
       <c r="F177" s="1">
         <v>6.0</v>
       </c>
-      <c r="K177" s="3">
-        <v>45840.0</v>
+      <c r="K177" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="178">
@@ -12714,8 +12719,8 @@
       <c r="F178" s="1">
         <v>9.0</v>
       </c>
-      <c r="K178" s="3">
-        <v>45840.0</v>
+      <c r="K178" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="179">
@@ -12737,8 +12742,8 @@
       <c r="F179" s="1">
         <v>4.0</v>
       </c>
-      <c r="K179" s="3">
-        <v>45840.0</v>
+      <c r="K179" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="180">
@@ -12760,8 +12765,8 @@
       <c r="F180" s="1">
         <v>6.0</v>
       </c>
-      <c r="K180" s="3">
-        <v>45840.0</v>
+      <c r="K180" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="181">
@@ -12783,8 +12788,8 @@
       <c r="F181" s="1">
         <v>13.0</v>
       </c>
-      <c r="K181" s="3">
-        <v>45840.0</v>
+      <c r="K181" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="182">
@@ -12806,8 +12811,8 @@
       <c r="F182" s="1">
         <v>8.0</v>
       </c>
-      <c r="K182" s="3">
-        <v>45840.0</v>
+      <c r="K182" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="183">
@@ -12829,8 +12834,8 @@
       <c r="F183" s="1">
         <v>14.0</v>
       </c>
-      <c r="K183" s="3">
-        <v>45840.0</v>
+      <c r="K183" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="184">
@@ -12838,10 +12843,10 @@
         <v>946.0</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K184" s="3">
-        <v>45840.0</v>
+        <v>89</v>
+      </c>
+      <c r="K184" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="185">
@@ -12849,10 +12854,10 @@
         <v>430.0</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K185" s="3">
-        <v>45840.0</v>
+        <v>89</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="186">
@@ -12860,10 +12865,10 @@
         <v>649.0</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K186" s="3">
-        <v>45840.0</v>
+        <v>89</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="187">
@@ -12871,10 +12876,10 @@
         <v>774.0</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K187" s="3">
-        <v>45840.0</v>
+        <v>89</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="188">
@@ -12882,10 +12887,10 @@
         <v>748.0</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K188" s="3">
-        <v>45840.0</v>
+        <v>89</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="189">
@@ -12907,8 +12912,8 @@
       <c r="F189" s="1">
         <v>6.0</v>
       </c>
-      <c r="K189" s="3">
-        <v>45840.0</v>
+      <c r="K189" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="190">
@@ -12933,8 +12938,8 @@
       <c r="J190" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K190" s="3">
-        <v>45840.0</v>
+      <c r="K190" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="192">
@@ -12956,8 +12961,8 @@
       <c r="F192" s="1">
         <v>4.0</v>
       </c>
-      <c r="K192" s="3">
-        <v>45846.0</v>
+      <c r="K192" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="193">
@@ -12979,8 +12984,8 @@
       <c r="F193" s="1">
         <v>0.0</v>
       </c>
-      <c r="K193" s="3">
-        <v>45846.0</v>
+      <c r="K193" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="194">
@@ -13002,8 +13007,8 @@
       <c r="F194" s="1">
         <v>3.0</v>
       </c>
-      <c r="K194" s="3">
-        <v>45846.0</v>
+      <c r="K194" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="195">
@@ -13025,8 +13030,8 @@
       <c r="F195" s="1">
         <v>5.0</v>
       </c>
-      <c r="K195" s="3">
-        <v>45846.0</v>
+      <c r="K195" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="196">
@@ -13048,8 +13053,8 @@
       <c r="F196" s="1">
         <v>3.0</v>
       </c>
-      <c r="K196" s="3">
-        <v>45846.0</v>
+      <c r="K196" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="197">
@@ -13071,8 +13076,8 @@
       <c r="F197" s="1">
         <v>6.0</v>
       </c>
-      <c r="K197" s="3">
-        <v>45846.0</v>
+      <c r="K197" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="198">
@@ -13094,8 +13099,8 @@
       <c r="F198" s="1">
         <v>0.0</v>
       </c>
-      <c r="K198" s="3">
-        <v>45846.0</v>
+      <c r="K198" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="199">
@@ -13117,8 +13122,8 @@
       <c r="F199" s="1">
         <v>4.0</v>
       </c>
-      <c r="K199" s="3">
-        <v>45846.0</v>
+      <c r="K199" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="200">
@@ -13140,8 +13145,8 @@
       <c r="F200" s="1">
         <v>11.0</v>
       </c>
-      <c r="K200" s="3">
-        <v>45846.0</v>
+      <c r="K200" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="201">
@@ -13151,8 +13156,8 @@
       <c r="J201" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K201" s="3">
-        <v>45846.0</v>
+      <c r="K201" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="202">
@@ -13174,8 +13179,8 @@
       <c r="F202" s="1">
         <v>3.0</v>
       </c>
-      <c r="K202" s="3">
-        <v>45846.0</v>
+      <c r="K202" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="203">
@@ -13197,8 +13202,8 @@
       <c r="F203" s="1">
         <v>6.0</v>
       </c>
-      <c r="K203" s="3">
-        <v>45846.0</v>
+      <c r="K203" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="204">
@@ -13208,8 +13213,8 @@
       <c r="J204" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K204" s="3">
-        <v>45846.0</v>
+      <c r="K204" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="205">
@@ -13219,8 +13224,8 @@
       <c r="J205" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K205" s="3">
-        <v>45846.0</v>
+      <c r="K205" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="206">
@@ -13242,8 +13247,8 @@
       <c r="F206" s="1">
         <v>2.0</v>
       </c>
-      <c r="K206" s="3">
-        <v>45846.0</v>
+      <c r="K206" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="207">
@@ -13265,8 +13270,8 @@
       <c r="F207" s="1">
         <v>9.0</v>
       </c>
-      <c r="K207" s="3">
-        <v>45846.0</v>
+      <c r="K207" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="208">
@@ -13288,8 +13293,8 @@
       <c r="F208" s="1">
         <v>7.0</v>
       </c>
-      <c r="K208" s="3">
-        <v>45846.0</v>
+      <c r="K208" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="209">
@@ -13299,8 +13304,8 @@
       <c r="J209" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K209" s="3">
-        <v>45846.0</v>
+      <c r="K209" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="210">
@@ -13310,8 +13315,8 @@
       <c r="J210" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K210" s="3">
-        <v>45846.0</v>
+      <c r="K210" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="211">
@@ -13333,8 +13338,8 @@
       <c r="F211" s="1">
         <v>6.0</v>
       </c>
-      <c r="K211" s="3">
-        <v>45846.0</v>
+      <c r="K211" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="212">
@@ -13356,8 +13361,8 @@
       <c r="F212" s="1">
         <v>2.0</v>
       </c>
-      <c r="K212" s="3">
-        <v>45846.0</v>
+      <c r="K212" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="213">
@@ -13379,8 +13384,8 @@
       <c r="F213" s="1">
         <v>3.0</v>
       </c>
-      <c r="K213" s="3">
-        <v>45846.0</v>
+      <c r="K213" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="214">
@@ -13390,8 +13395,8 @@
       <c r="J214" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K214" s="3">
-        <v>45846.0</v>
+      <c r="K214" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="215">
@@ -13413,8 +13418,8 @@
       <c r="F215" s="1">
         <v>3.0</v>
       </c>
-      <c r="K215" s="3">
-        <v>45846.0</v>
+      <c r="K215" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="216">
@@ -13424,8 +13429,8 @@
       <c r="J216" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K216" s="3">
-        <v>45846.0</v>
+      <c r="K216" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="217">
@@ -13447,8 +13452,8 @@
       <c r="F217" s="1">
         <v>6.0</v>
       </c>
-      <c r="K217" s="3">
-        <v>45846.0</v>
+      <c r="K217" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="218">
@@ -13474,13 +13479,13 @@
         <v>10.9</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K218" s="3">
-        <v>45846.0</v>
+        <v>84</v>
+      </c>
+      <c r="K218" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="219">
@@ -13502,8 +13507,8 @@
       <c r="F219" s="1">
         <v>3.0</v>
       </c>
-      <c r="K219" s="3">
-        <v>45846.0</v>
+      <c r="K219" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="220">
@@ -13513,8 +13518,8 @@
       <c r="J220" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K220" s="3">
-        <v>45846.0</v>
+      <c r="K220" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="221">
@@ -13524,8 +13529,8 @@
       <c r="J221" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K221" s="3">
-        <v>45846.0</v>
+      <c r="K221" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="222">
@@ -13535,8 +13540,8 @@
       <c r="J222" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K222" s="3">
-        <v>45846.0</v>
+      <c r="K222" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="223">
@@ -13558,8 +13563,8 @@
       <c r="F223" s="1">
         <v>11.0</v>
       </c>
-      <c r="K223" s="3">
-        <v>45846.0</v>
+      <c r="K223" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="224">
@@ -13581,8 +13586,8 @@
       <c r="F224" s="1">
         <v>2.0</v>
       </c>
-      <c r="K224" s="3">
-        <v>45846.0</v>
+      <c r="K224" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="225">
@@ -13604,8 +13609,8 @@
       <c r="F225" s="1">
         <v>4.0</v>
       </c>
-      <c r="K225" s="3">
-        <v>45846.0</v>
+      <c r="K225" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="226">
@@ -13615,8 +13620,8 @@
       <c r="J226" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K226" s="3">
-        <v>45846.0</v>
+      <c r="K226" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="227">
@@ -13626,8 +13631,8 @@
       <c r="J227" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K227" s="3">
-        <v>45846.0</v>
+      <c r="K227" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="228">
@@ -13649,8 +13654,8 @@
       <c r="F228" s="1">
         <v>7.0</v>
       </c>
-      <c r="K228" s="3">
-        <v>45846.0</v>
+      <c r="K228" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="229">
@@ -13660,8 +13665,8 @@
       <c r="J229" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K229" s="3">
-        <v>45846.0</v>
+      <c r="K229" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="230">
@@ -13671,8 +13676,8 @@
       <c r="J230" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K230" s="3">
-        <v>45846.0</v>
+      <c r="K230" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="231">
@@ -13694,8 +13699,8 @@
       <c r="F231" s="1">
         <v>9.0</v>
       </c>
-      <c r="K231" s="3">
-        <v>45846.0</v>
+      <c r="K231" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="232">
@@ -13717,8 +13722,8 @@
       <c r="F232" s="1">
         <v>6.0</v>
       </c>
-      <c r="K232" s="3">
-        <v>45846.0</v>
+      <c r="K232" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="233">
@@ -13728,8 +13733,8 @@
       <c r="J233" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K233" s="3">
-        <v>45846.0</v>
+      <c r="K233" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="234">
@@ -13751,8 +13756,8 @@
       <c r="F234" s="1">
         <v>4.0</v>
       </c>
-      <c r="K234" s="3">
-        <v>45846.0</v>
+      <c r="K234" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="235">
@@ -13774,8 +13779,8 @@
       <c r="F235" s="1">
         <v>7.0</v>
       </c>
-      <c r="K235" s="3">
-        <v>45846.0</v>
+      <c r="K235" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="236">
@@ -13785,8 +13790,8 @@
       <c r="J236" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K236" s="3">
-        <v>45846.0</v>
+      <c r="K236" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="237">
@@ -13808,8 +13813,8 @@
       <c r="F237" s="1">
         <v>6.0</v>
       </c>
-      <c r="K237" s="3">
-        <v>45846.0</v>
+      <c r="K237" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="238">
@@ -13831,8 +13836,8 @@
       <c r="F238" s="1">
         <v>3.0</v>
       </c>
-      <c r="K238" s="3">
-        <v>45846.0</v>
+      <c r="K238" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="239">
@@ -13858,13 +13863,13 @@
         <v>4.16</v>
       </c>
       <c r="H239" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K239" s="3">
-        <v>45846.0</v>
+        <v>75</v>
+      </c>
+      <c r="K239" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="240">
@@ -13886,8 +13891,8 @@
       <c r="F240" s="1">
         <v>4.0</v>
       </c>
-      <c r="K240" s="3">
-        <v>45846.0</v>
+      <c r="K240" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="241">
@@ -13913,13 +13918,13 @@
         <v>6.25</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I241" s="1">
         <v>3.0</v>
       </c>
-      <c r="K241" s="3">
-        <v>45846.0</v>
+      <c r="K241" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="242">
@@ -13941,8 +13946,8 @@
       <c r="F242" s="1">
         <v>6.0</v>
       </c>
-      <c r="K242" s="3">
-        <v>45846.0</v>
+      <c r="K242" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="243">
@@ -13964,8 +13969,8 @@
       <c r="F243" s="1">
         <v>9.0</v>
       </c>
-      <c r="K243" s="3">
-        <v>45846.0</v>
+      <c r="K243" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="244">
@@ -13987,8 +13992,8 @@
       <c r="F244" s="1">
         <v>0.0</v>
       </c>
-      <c r="K244" s="3">
-        <v>45846.0</v>
+      <c r="K244" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="245">
@@ -14010,8 +14015,8 @@
       <c r="F245" s="1">
         <v>10.0</v>
       </c>
-      <c r="K245" s="3">
-        <v>45846.0</v>
+      <c r="K245" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="246">
@@ -14033,8 +14038,8 @@
       <c r="F246" s="1">
         <v>2.0</v>
       </c>
-      <c r="K246" s="3">
-        <v>45846.0</v>
+      <c r="K246" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="247">
@@ -14060,13 +14065,13 @@
         <v>6.25</v>
       </c>
       <c r="H247" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I247" s="1">
         <v>2.0</v>
       </c>
-      <c r="K247" s="3">
-        <v>45846.0</v>
+      <c r="K247" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="248">
@@ -14089,13 +14094,13 @@
         <v>8.0</v>
       </c>
       <c r="H248" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I248" s="1">
         <v>2.0</v>
       </c>
-      <c r="K248" s="3">
-        <v>45846.0</v>
+      <c r="K248" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="249">
@@ -14117,8 +14122,8 @@
       <c r="F249" s="1">
         <v>6.0</v>
       </c>
-      <c r="K249" s="3">
-        <v>45846.0</v>
+      <c r="K249" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="250">
@@ -14144,13 +14149,13 @@
         <v>4.4</v>
       </c>
       <c r="H250" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I250" s="1">
         <v>2.0</v>
       </c>
-      <c r="K250" s="3">
-        <v>45846.0</v>
+      <c r="K250" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="251">
@@ -14172,8 +14177,8 @@
       <c r="F251" s="1">
         <v>9.0</v>
       </c>
-      <c r="K251" s="3">
-        <v>45846.0</v>
+      <c r="K251" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="252">
@@ -14195,8 +14200,8 @@
       <c r="F252" s="1">
         <v>6.0</v>
       </c>
-      <c r="K252" s="3">
-        <v>45846.0</v>
+      <c r="K252" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="253">
@@ -14222,10 +14227,10 @@
         <v>4.54</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K253" s="3">
-        <v>45846.0</v>
+        <v>79</v>
+      </c>
+      <c r="K253" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="254">
@@ -14247,8 +14252,8 @@
       <c r="F254" s="1">
         <v>8.0</v>
       </c>
-      <c r="K254" s="3">
-        <v>45846.0</v>
+      <c r="K254" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="255">
@@ -14274,13 +14279,13 @@
         <v>3.07</v>
       </c>
       <c r="H255" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K255" s="3">
-        <v>45846.0</v>
+        <v>92</v>
+      </c>
+      <c r="K255" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="256">
@@ -14303,13 +14308,13 @@
         <v>5.0</v>
       </c>
       <c r="H256" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I256" s="1">
         <v>3.0</v>
       </c>
-      <c r="K256" s="3">
-        <v>45846.0</v>
+      <c r="K256" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="258">
@@ -14322,8 +14327,8 @@
       <c r="D258" s="1">
         <v>8.0</v>
       </c>
-      <c r="K258" s="3">
-        <v>45855.0</v>
+      <c r="K258" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="259">
@@ -14333,8 +14338,8 @@
       <c r="B259" s="1">
         <v>8.0</v>
       </c>
-      <c r="K259" s="3">
-        <v>45855.0</v>
+      <c r="K259" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="260">
@@ -14344,8 +14349,8 @@
       <c r="B260" s="1">
         <v>3.5</v>
       </c>
-      <c r="K260" s="3">
-        <v>45855.0</v>
+      <c r="K260" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="261">
@@ -14355,8 +14360,8 @@
       <c r="B261" s="1">
         <v>4.0</v>
       </c>
-      <c r="K261" s="3">
-        <v>45855.0</v>
+      <c r="K261" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="262">
@@ -14369,8 +14374,8 @@
       <c r="D262" s="1">
         <v>7.0</v>
       </c>
-      <c r="K262" s="3">
-        <v>45855.0</v>
+      <c r="K262" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="263">
@@ -14383,8 +14388,8 @@
       <c r="D263" s="1">
         <v>3.0</v>
       </c>
-      <c r="K263" s="3">
-        <v>45855.0</v>
+      <c r="K263" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="264">
@@ -14397,8 +14402,8 @@
       <c r="D264" s="1">
         <v>9.0</v>
       </c>
-      <c r="K264" s="3">
-        <v>45855.0</v>
+      <c r="K264" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="265">
@@ -14411,8 +14416,8 @@
       <c r="D265" s="1">
         <v>1.0</v>
       </c>
-      <c r="K265" s="3">
-        <v>45855.0</v>
+      <c r="K265" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="266">
@@ -14425,8 +14430,8 @@
       <c r="D266" s="1">
         <v>1.0</v>
       </c>
-      <c r="K266" s="3">
-        <v>45855.0</v>
+      <c r="K266" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="267">
@@ -14434,10 +14439,10 @@
         <v>762.0</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K267" s="3">
-        <v>45855.0</v>
+        <v>94</v>
+      </c>
+      <c r="K267" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="268">
@@ -14450,8 +14455,8 @@
       <c r="D268" s="1">
         <v>2.0</v>
       </c>
-      <c r="K268" s="3">
-        <v>45855.0</v>
+      <c r="K268" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="269">
@@ -14464,8 +14469,8 @@
       <c r="D269" s="1">
         <v>1.0</v>
       </c>
-      <c r="K269" s="3">
-        <v>45855.0</v>
+      <c r="K269" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="270">
@@ -14487,8 +14492,8 @@
       <c r="F270" s="1">
         <v>7.0</v>
       </c>
-      <c r="K270" s="3">
-        <v>45855.0</v>
+      <c r="K270" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="271">
@@ -14501,8 +14506,8 @@
       <c r="D271" s="1">
         <v>3.0</v>
       </c>
-      <c r="K271" s="3">
-        <v>45855.0</v>
+      <c r="K271" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="272">
@@ -14515,8 +14520,8 @@
       <c r="D272" s="1">
         <v>6.0</v>
       </c>
-      <c r="K272" s="3">
-        <v>45855.0</v>
+      <c r="K272" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="273">
@@ -14524,10 +14529,10 @@
         <v>412.0</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K273" s="3">
-        <v>45855.0</v>
+        <v>94</v>
+      </c>
+      <c r="K273" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="274">
@@ -14535,10 +14540,10 @@
         <v>430.0</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K274" s="3">
-        <v>45855.0</v>
+        <v>94</v>
+      </c>
+      <c r="K274" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="275">
@@ -14551,8 +14556,8 @@
       <c r="D275" s="1">
         <v>3.0</v>
       </c>
-      <c r="K275" s="3">
-        <v>45855.0</v>
+      <c r="K275" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="276">
@@ -14565,8 +14570,8 @@
       <c r="D276" s="1">
         <v>1.0</v>
       </c>
-      <c r="K276" s="3">
-        <v>45855.0</v>
+      <c r="K276" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="277">
@@ -14574,10 +14579,10 @@
         <v>248.0</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K277" s="3">
-        <v>45855.0</v>
+        <v>94</v>
+      </c>
+      <c r="K277" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="278">
@@ -14590,8 +14595,8 @@
       <c r="D278" s="1">
         <v>1.0</v>
       </c>
-      <c r="K278" s="3">
-        <v>45855.0</v>
+      <c r="K278" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="279">
@@ -14613,8 +14618,8 @@
       <c r="F279" s="1">
         <v>6.0</v>
       </c>
-      <c r="K279" s="3">
-        <v>45855.0</v>
+      <c r="K279" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="280">
@@ -14627,8 +14632,8 @@
       <c r="D280" s="1">
         <v>1.0</v>
       </c>
-      <c r="K280" s="3">
-        <v>45855.0</v>
+      <c r="K280" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="281">
@@ -14650,8 +14655,8 @@
       <c r="F281" s="1">
         <v>6.0</v>
       </c>
-      <c r="K281" s="3">
-        <v>45855.0</v>
+      <c r="K281" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="282">
@@ -14664,8 +14669,8 @@
       <c r="D282" s="1">
         <v>4.0</v>
       </c>
-      <c r="K282" s="3">
-        <v>45855.0</v>
+      <c r="K282" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="283">
@@ -14681,8 +14686,8 @@
       <c r="F283" s="1">
         <v>3.0</v>
       </c>
-      <c r="K283" s="3">
-        <v>45855.0</v>
+      <c r="K283" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="284">
@@ -14695,8 +14700,8 @@
       <c r="D284" s="1">
         <v>2.0</v>
       </c>
-      <c r="K284" s="3">
-        <v>45855.0</v>
+      <c r="K284" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="285">
@@ -14718,8 +14723,8 @@
       <c r="F285" s="1">
         <v>8.0</v>
       </c>
-      <c r="K285" s="3">
-        <v>45855.0</v>
+      <c r="K285" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="286">
@@ -14732,8 +14737,8 @@
       <c r="E286" s="1">
         <v>1.0</v>
       </c>
-      <c r="K286" s="3">
-        <v>45855.0</v>
+      <c r="K286" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="287">
@@ -14749,8 +14754,8 @@
       <c r="F287" s="1">
         <v>8.0</v>
       </c>
-      <c r="K287" s="3">
-        <v>45855.0</v>
+      <c r="K287" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="288">
@@ -14763,8 +14768,8 @@
       <c r="D288" s="1">
         <v>3.0</v>
       </c>
-      <c r="K288" s="3">
-        <v>45855.0</v>
+      <c r="K288" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="289">
@@ -14787,10 +14792,10 @@
         <v>6.0</v>
       </c>
       <c r="J289" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K289" s="3">
-        <v>45855.0</v>
+        <v>95</v>
+      </c>
+      <c r="K289" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="290">
@@ -14803,23 +14808,23 @@
       <c r="D290" s="1">
         <v>1.0</v>
       </c>
-      <c r="K290" s="3">
-        <v>45855.0</v>
+      <c r="K290" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="6">
+      <c r="A291" s="5">
         <v>922.0</v>
       </c>
-      <c r="B291" s="6">
+      <c r="B291" s="5">
         <v>7.5</v>
       </c>
-      <c r="C291" s="7"/>
-      <c r="D291" s="6">
+      <c r="C291" s="6"/>
+      <c r="D291" s="5">
         <v>7.0</v>
       </c>
-      <c r="K291" s="3">
-        <v>45855.0</v>
+      <c r="K291" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="292">
@@ -14832,8 +14837,8 @@
       <c r="D292" s="1">
         <v>6.0</v>
       </c>
-      <c r="K292" s="3">
-        <v>45855.0</v>
+      <c r="K292" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="293">
@@ -14855,8 +14860,8 @@
       <c r="F293" s="1">
         <v>9.0</v>
       </c>
-      <c r="K293" s="3">
-        <v>45855.0</v>
+      <c r="K293" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="294">
@@ -14878,8 +14883,8 @@
       <c r="F294" s="1">
         <v>7.0</v>
       </c>
-      <c r="K294" s="3">
-        <v>45855.0</v>
+      <c r="K294" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="295">
@@ -14892,8 +14897,8 @@
       <c r="D295" s="1">
         <v>1.0</v>
       </c>
-      <c r="K295" s="3">
-        <v>45855.0</v>
+      <c r="K295" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="296">
@@ -14906,8 +14911,8 @@
       <c r="D296" s="1">
         <v>3.0</v>
       </c>
-      <c r="K296" s="3">
-        <v>45855.0</v>
+      <c r="K296" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="297">
@@ -14920,8 +14925,8 @@
       <c r="D297" s="1">
         <v>4.0</v>
       </c>
-      <c r="K297" s="3">
-        <v>45855.0</v>
+      <c r="K297" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="298">
@@ -14940,8 +14945,8 @@
       <c r="F298" s="1">
         <v>6.0</v>
       </c>
-      <c r="K298" s="3">
-        <v>45855.0</v>
+      <c r="K298" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="299">
@@ -14963,8 +14968,8 @@
       <c r="F299" s="1">
         <v>12.0</v>
       </c>
-      <c r="K299" s="3">
-        <v>45855.0</v>
+      <c r="K299" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="300">
@@ -14977,8 +14982,8 @@
       <c r="D300" s="1">
         <v>3.0</v>
       </c>
-      <c r="K300" s="3">
-        <v>45855.0</v>
+      <c r="K300" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="301">
@@ -15000,8 +15005,8 @@
       <c r="F301" s="1">
         <v>16.0</v>
       </c>
-      <c r="K301" s="3">
-        <v>45855.0</v>
+      <c r="K301" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="302">
@@ -15014,8 +15019,8 @@
       <c r="D302" s="1">
         <v>1.0</v>
       </c>
-      <c r="K302" s="3">
-        <v>45855.0</v>
+      <c r="K302" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="303">
@@ -15028,8 +15033,8 @@
       <c r="D303" s="1">
         <v>4.0</v>
       </c>
-      <c r="K303" s="3">
-        <v>45855.0</v>
+      <c r="K303" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="305">
@@ -15052,10 +15057,10 @@
         <v>6.0</v>
       </c>
       <c r="J305" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K305" s="8">
-        <v>45860.0</v>
+        <v>96</v>
+      </c>
+      <c r="K305" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="306">
@@ -15068,17 +15073,17 @@
       <c r="C306" s="1">
         <v>1.25</v>
       </c>
-      <c r="D306" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="E306" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="F306" s="6">
+      <c r="D306" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E306" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F306" s="5">
         <v>4.0</v>
       </c>
-      <c r="K306" s="8">
-        <v>45860.0</v>
+      <c r="K306" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="307">
@@ -15101,10 +15106,10 @@
         <v>5.0</v>
       </c>
       <c r="J307" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K307" s="8">
-        <v>45860.0</v>
+        <v>98</v>
+      </c>
+      <c r="K307" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="308">
@@ -15126,8 +15131,8 @@
       <c r="F308" s="1">
         <v>6.0</v>
       </c>
-      <c r="K308" s="8">
-        <v>45860.0</v>
+      <c r="K308" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="309">
@@ -15147,10 +15152,10 @@
         <v>0.0</v>
       </c>
       <c r="J309" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K309" s="8">
-        <v>45860.0</v>
+        <v>98</v>
+      </c>
+      <c r="K309" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="310">
@@ -15173,10 +15178,10 @@
         <v>7.0</v>
       </c>
       <c r="J310" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K310" s="8">
-        <v>45860.0</v>
+        <v>98</v>
+      </c>
+      <c r="K310" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="311">
@@ -15198,8 +15203,8 @@
       <c r="F311" s="1">
         <v>6.0</v>
       </c>
-      <c r="K311" s="8">
-        <v>45860.0</v>
+      <c r="K311" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="312">
@@ -15222,10 +15227,10 @@
         <v>6.0</v>
       </c>
       <c r="J312" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K312" s="8">
-        <v>45860.0</v>
+        <v>98</v>
+      </c>
+      <c r="K312" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="313">
@@ -15248,10 +15253,10 @@
         <v>8.0</v>
       </c>
       <c r="J313" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K313" s="8">
-        <v>45860.0</v>
+        <v>99</v>
+      </c>
+      <c r="K313" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="314">
@@ -15273,8 +15278,8 @@
       <c r="F314" s="1">
         <v>7.0</v>
       </c>
-      <c r="K314" s="8">
-        <v>45860.0</v>
+      <c r="K314" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="315">
@@ -15296,8 +15301,8 @@
       <c r="F315" s="1">
         <v>16.0</v>
       </c>
-      <c r="K315" s="8">
-        <v>45860.0</v>
+      <c r="K315" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="317">
@@ -15325,7 +15330,7 @@
         <v>667.0</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="319">

</xml_diff>

<commit_message>
fixed dates some more in xlsx
</commit_message>
<xml_diff>
--- a/data/Moser creek data.xlsx
+++ b/data/Moser creek data.xlsx
@@ -217,7 +217,7 @@
     <t>EFN_score</t>
   </si>
   <si>
-    <t>6.25.25</t>
+    <t>6.25.2025</t>
   </si>
   <si>
     <t>e no mv</t>
@@ -277,7 +277,7 @@
     <t>e + mv</t>
   </si>
   <si>
-    <t>7.2.25</t>
+    <t>7.2.2025</t>
   </si>
   <si>
     <t>whole leaf</t>
@@ -289,7 +289,7 @@
     <t>dug up</t>
   </si>
   <si>
-    <t>7.8.25</t>
+    <t>7.8.2025</t>
   </si>
   <si>
     <t>e w mv</t>
@@ -298,7 +298,7 @@
     <t>4,5</t>
   </si>
   <si>
-    <t>7.17.25</t>
+    <t>7.17.2025</t>
   </si>
   <si>
     <t>NA</t>
@@ -310,7 +310,7 @@
     <t>DEAD top eaten</t>
   </si>
   <si>
-    <t>7.22.25</t>
+    <t>7.22.2025</t>
   </si>
   <si>
     <t>DEAD</t>

</xml_diff>